<commit_message>
Spikes_stable better graphics; some fun with shaders ("better" "blur", clouds)
</commit_message>
<xml_diff>
--- a/Wiki/Gameplay/World/Enemies.xlsx
+++ b/Wiki/Gameplay/World/Enemies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Normal" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>HP</t>
   </si>
@@ -86,6 +86,9 @@
   <si>
     <t>Gets stunned if hits the wall
 Can be hit only from behind</t>
+  </si>
+  <si>
+    <t>Wall walker</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q14"/>
+  <dimension ref="A2:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,6 +693,14 @@
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>